<commit_message>
Atualizacao Grafico de Burndown dos sprints
</commit_message>
<xml_diff>
--- a/academicci_documentacao/gerencia_projeto/Academicci_GBS_BurndownSprint.xlsx
+++ b/academicci_documentacao/gerencia_projeto/Academicci_GBS_BurndownSprint.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\Google Drive\University - Atividades e Trabalhos\PFS_II\repositorio\documentacao\processo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\Google Drive\University - Atividades e Trabalhos\PFS_II\Academicci_II\academicci_documentacao\gerencia_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7770" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Grafico" sheetId="2" r:id="rId1"/>
-    <sheet name="Dados" sheetId="1" r:id="rId2"/>
+    <sheet name="Sprint01" sheetId="2" r:id="rId1"/>
+    <sheet name="Sprint02" sheetId="3" r:id="rId2"/>
+    <sheet name="Dados" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Dia 01</t>
   </si>
@@ -136,13 +137,52 @@
   </si>
   <si>
     <t>01</t>
+  </si>
+  <si>
+    <t>Realizar Login</t>
+  </si>
+  <si>
+    <t>Candidatar a Monitor</t>
+  </si>
+  <si>
+    <t>Dia 31</t>
+  </si>
+  <si>
+    <t>Dia 32</t>
+  </si>
+  <si>
+    <t>Dia 33</t>
+  </si>
+  <si>
+    <t>Dia 34</t>
+  </si>
+  <si>
+    <t>Dia 35</t>
+  </si>
+  <si>
+    <t>Dia 36</t>
+  </si>
+  <si>
+    <t>Dia 37</t>
+  </si>
+  <si>
+    <t>Dia 38</t>
+  </si>
+  <si>
+    <t>Dia 39</t>
+  </si>
+  <si>
+    <t>Dia 40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +233,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -226,7 +272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -273,11 +319,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -287,13 +370,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -316,6 +393,28 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,7 +516,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dados!$B$4</c:f>
+              <c:f>Dados!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -442,99 +541,129 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Dados!$D$4:$AG$4</c:f>
+              <c:f>Dados!$D$6:$AQ$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -551,7 +680,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dados!$B$5</c:f>
+              <c:f>Dados!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -575,99 +704,129 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Dados!$D$5:$AG$5</c:f>
+              <c:f>Dados!$D$7:$AQ$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>9.6666666666666661</c:v>
+                  <c:v>22.425000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3333333333333321</c:v>
+                  <c:v>21.85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.9999999999999982</c:v>
+                  <c:v>21.275000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.6666666666666643</c:v>
+                  <c:v>20.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.3333333333333304</c:v>
+                  <c:v>20.125000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.9999999999999973</c:v>
+                  <c:v>19.550000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.6666666666666643</c:v>
+                  <c:v>18.975000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.3333333333333313</c:v>
+                  <c:v>18.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.9999999999999982</c:v>
+                  <c:v>17.825000000000006</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.6666666666666652</c:v>
+                  <c:v>17.250000000000007</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.3333333333333321</c:v>
+                  <c:v>16.675000000000008</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.9999999999999991</c:v>
+                  <c:v>16.100000000000009</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.6666666666666661</c:v>
+                  <c:v>15.525000000000009</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.333333333333333</c:v>
+                  <c:v>14.95000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5</c:v>
+                  <c:v>14.375000000000011</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.666666666666667</c:v>
+                  <c:v>13.800000000000011</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.3333333333333339</c:v>
+                  <c:v>13.225000000000012</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.0000000000000009</c:v>
+                  <c:v>12.650000000000013</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.6666666666666674</c:v>
+                  <c:v>12.075000000000014</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.3333333333333339</c:v>
+                  <c:v>11.500000000000014</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.0000000000000004</c:v>
+                  <c:v>10.925000000000015</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.666666666666667</c:v>
+                  <c:v>10.350000000000016</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.3333333333333335</c:v>
+                  <c:v>9.7750000000000163</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2</c:v>
+                  <c:v>9.2000000000000171</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.6666666666666667</c:v>
+                  <c:v>8.6250000000000178</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.3333333333333335</c:v>
+                  <c:v>8.0500000000000185</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.0000000000000002</c:v>
+                  <c:v>7.4750000000000183</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.66666666666666696</c:v>
+                  <c:v>6.9000000000000181</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.33333333333333365</c:v>
+                  <c:v>6.3250000000000179</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>5.7500000000000178</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.1750000000000176</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.6000000000000174</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.0250000000000172</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.4500000000000171</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.8750000000000169</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.3000000000000167</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.7250000000000167</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.1500000000000168</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.57500000000001683</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.6875389974302379E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -888,7 +1047,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -923,6 +1082,578 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Gráfico BurnDown - Sprint 02</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dados!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Restantes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Dados!$D$11:$R$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8CB6-46DD-87A7-77FEA2980EB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dados!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Estimadas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Dados!$D$12:$R$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>9.3333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.6666666666666679</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0000000000000018</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3333333333333348</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6666666666666679</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.6666666666666673</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8CB6-46DD-87A7-77FEA2980EB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="778639600"/>
+        <c:axId val="778635856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="778639600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" b="1">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Dias</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="778635856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="778635856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="12"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" b="1">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Hoaras</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="778639600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1040,7 +1771,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1568,6 +2842,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180973</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACFE61B1-19C7-4FED-A857-23140CA48041}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1850,7 +3167,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,7 +3176,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
+      <c r="A1" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1869,10 +3186,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AQ12"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,7 +3223,7 @@
     <col min="44" max="63" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
@@ -1984,16 +3323,46 @@
       <c r="AG1" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="AH1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:43" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="12">
-        <v>10</v>
+      <c r="C2" s="10">
+        <v>5</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -2012,7 +3381,9 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
+      <c r="U2" s="4">
+        <v>2</v>
+      </c>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
@@ -2025,303 +3396,699 @@
       <c r="AE2" s="4"/>
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4">
+        <v>3</v>
+      </c>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="4"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="16"/>
-      <c r="AA3" s="16"/>
-      <c r="AB3" s="16"/>
-      <c r="AC3" s="16"/>
-      <c r="AD3" s="16"/>
-      <c r="AE3" s="16"/>
-      <c r="AF3" s="16"/>
-      <c r="AG3" s="16"/>
+    <row r="3" spans="1:43" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="22"/>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="10">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4">
+        <v>4</v>
+      </c>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="4"/>
+      <c r="AP3" s="4">
+        <v>4</v>
+      </c>
+      <c r="AQ3" s="4"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="1:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="10">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4">
+        <v>5</v>
+      </c>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="4"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="14"/>
+      <c r="AH5" s="14"/>
+      <c r="AI5" s="14"/>
+      <c r="AJ5" s="14"/>
+      <c r="AK5" s="14"/>
+      <c r="AL5" s="14"/>
+      <c r="AM5" s="14"/>
+      <c r="AN5" s="14"/>
+      <c r="AO5" s="14"/>
+      <c r="AP5" s="14"/>
+      <c r="AQ5" s="14"/>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+      <c r="B6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="10">
-        <f>SUM(C2:C2)</f>
+      <c r="C6" s="8">
+        <f>SUM(C2:C4)</f>
+        <v>23</v>
+      </c>
+      <c r="D6" s="20">
+        <f>C6-SUM(D2:D4)</f>
+        <v>23</v>
+      </c>
+      <c r="E6" s="20">
+        <f t="shared" ref="E6:AG6" si="0">D6-SUM(E2:E4)</f>
+        <v>23</v>
+      </c>
+      <c r="F6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="G6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="H6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="I6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="J6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="K6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="L6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="M6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="N6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="O6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="P6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="Q6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="R6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="S6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="T6" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="U6" s="20">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="V6" s="20">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="W6" s="20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="X6" s="20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Y6" s="20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Z6" s="20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AA6" s="20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AB6" s="20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AC6" s="20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AD6" s="20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AE6" s="20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AF6" s="20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AG6" s="20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AH6" s="20">
+        <f t="shared" ref="AH6:AQ6" si="1">AG6-SUM(AH2:AH4)</f>
+        <v>12</v>
+      </c>
+      <c r="AI6" s="20">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="AJ6" s="20">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="AK6" s="20">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="AL6" s="20">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="AM6" s="20">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="AN6" s="20">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="AO6" s="20">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="AP6" s="20">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AQ6" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
+      <c r="B7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="19">
+        <v>23</v>
+      </c>
+      <c r="D7" s="18">
+        <f>C7-($C$7/COUNTA($D$1:$AQ$1))</f>
+        <v>22.425000000000001</v>
+      </c>
+      <c r="E7" s="18">
+        <f t="shared" ref="E7:AQ7" si="2">D7-($C$7/COUNTA($D$1:$AQ$1))</f>
+        <v>21.85</v>
+      </c>
+      <c r="F7" s="18">
+        <f t="shared" si="2"/>
+        <v>21.275000000000002</v>
+      </c>
+      <c r="G7" s="18">
+        <f t="shared" si="2"/>
+        <v>20.700000000000003</v>
+      </c>
+      <c r="H7" s="18">
+        <f t="shared" si="2"/>
+        <v>20.125000000000004</v>
+      </c>
+      <c r="I7" s="18">
+        <f t="shared" si="2"/>
+        <v>19.550000000000004</v>
+      </c>
+      <c r="J7" s="18">
+        <f t="shared" si="2"/>
+        <v>18.975000000000005</v>
+      </c>
+      <c r="K7" s="18">
+        <f t="shared" si="2"/>
+        <v>18.400000000000006</v>
+      </c>
+      <c r="L7" s="18">
+        <f t="shared" si="2"/>
+        <v>17.825000000000006</v>
+      </c>
+      <c r="M7" s="18">
+        <f t="shared" si="2"/>
+        <v>17.250000000000007</v>
+      </c>
+      <c r="N7" s="18">
+        <f t="shared" si="2"/>
+        <v>16.675000000000008</v>
+      </c>
+      <c r="O7" s="18">
+        <f t="shared" si="2"/>
+        <v>16.100000000000009</v>
+      </c>
+      <c r="P7" s="18">
+        <f t="shared" si="2"/>
+        <v>15.525000000000009</v>
+      </c>
+      <c r="Q7" s="18">
+        <f t="shared" si="2"/>
+        <v>14.95000000000001</v>
+      </c>
+      <c r="R7" s="18">
+        <f t="shared" si="2"/>
+        <v>14.375000000000011</v>
+      </c>
+      <c r="S7" s="18">
+        <f t="shared" si="2"/>
+        <v>13.800000000000011</v>
+      </c>
+      <c r="T7" s="18">
+        <f t="shared" si="2"/>
+        <v>13.225000000000012</v>
+      </c>
+      <c r="U7" s="18">
+        <f t="shared" si="2"/>
+        <v>12.650000000000013</v>
+      </c>
+      <c r="V7" s="18">
+        <f t="shared" si="2"/>
+        <v>12.075000000000014</v>
+      </c>
+      <c r="W7" s="18">
+        <f t="shared" si="2"/>
+        <v>11.500000000000014</v>
+      </c>
+      <c r="X7" s="18">
+        <f t="shared" si="2"/>
+        <v>10.925000000000015</v>
+      </c>
+      <c r="Y7" s="18">
+        <f t="shared" si="2"/>
+        <v>10.350000000000016</v>
+      </c>
+      <c r="Z7" s="18">
+        <f t="shared" si="2"/>
+        <v>9.7750000000000163</v>
+      </c>
+      <c r="AA7" s="18">
+        <f t="shared" si="2"/>
+        <v>9.2000000000000171</v>
+      </c>
+      <c r="AB7" s="18">
+        <f t="shared" si="2"/>
+        <v>8.6250000000000178</v>
+      </c>
+      <c r="AC7" s="18">
+        <f t="shared" si="2"/>
+        <v>8.0500000000000185</v>
+      </c>
+      <c r="AD7" s="18">
+        <f t="shared" si="2"/>
+        <v>7.4750000000000183</v>
+      </c>
+      <c r="AE7" s="18">
+        <f t="shared" si="2"/>
+        <v>6.9000000000000181</v>
+      </c>
+      <c r="AF7" s="18">
+        <f t="shared" si="2"/>
+        <v>6.3250000000000179</v>
+      </c>
+      <c r="AG7" s="18">
+        <f t="shared" si="2"/>
+        <v>5.7500000000000178</v>
+      </c>
+      <c r="AH7" s="18">
+        <f t="shared" si="2"/>
+        <v>5.1750000000000176</v>
+      </c>
+      <c r="AI7" s="18">
+        <f t="shared" si="2"/>
+        <v>4.6000000000000174</v>
+      </c>
+      <c r="AJ7" s="18">
+        <f t="shared" si="2"/>
+        <v>4.0250000000000172</v>
+      </c>
+      <c r="AK7" s="18">
+        <f t="shared" si="2"/>
+        <v>3.4500000000000171</v>
+      </c>
+      <c r="AL7" s="18">
+        <f t="shared" si="2"/>
+        <v>2.8750000000000169</v>
+      </c>
+      <c r="AM7" s="18">
+        <f t="shared" si="2"/>
+        <v>2.3000000000000167</v>
+      </c>
+      <c r="AN7" s="18">
+        <f t="shared" si="2"/>
+        <v>1.7250000000000167</v>
+      </c>
+      <c r="AO7" s="18">
+        <f t="shared" si="2"/>
+        <v>1.1500000000000168</v>
+      </c>
+      <c r="AP7" s="18">
+        <f t="shared" si="2"/>
+        <v>0.57500000000001683</v>
+      </c>
+      <c r="AQ7" s="18">
+        <f t="shared" si="2"/>
+        <v>1.6875389974302379E-14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="10">
         <v>10</v>
       </c>
-      <c r="D4" s="7">
-        <f>C4-SUM(D2:D3)</f>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="8">
+        <f>SUM(C9:C9)</f>
         <v>10</v>
       </c>
-      <c r="E4" s="7">
-        <f>D4-SUM(E2:E3)</f>
+      <c r="D11" s="20">
+        <f>C11-SUM(D9)</f>
         <v>10</v>
       </c>
-      <c r="F4" s="7">
-        <f>E4-SUM(F2:F3)</f>
+      <c r="E11" s="20">
+        <f t="shared" ref="E11:R11" si="3">D11-SUM(E9)</f>
         <v>10</v>
       </c>
-      <c r="G4" s="7">
-        <f>F4-SUM(G2:G3)</f>
+      <c r="F11" s="20">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="H4" s="7">
-        <f>G4-SUM(H2:H3)</f>
+      <c r="G11" s="20">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="I4" s="7">
-        <f>H4-SUM(I2:I3)</f>
+      <c r="H11" s="20">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="J4" s="7">
-        <f>I4-SUM(J2:J3)</f>
+      <c r="I11" s="20">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="K4" s="7">
-        <f>J4-SUM(K2:K3)</f>
+      <c r="J11" s="20">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="L4" s="7">
-        <f>K4-SUM(L2:L3)</f>
+      <c r="K11" s="20">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="M4" s="7">
-        <f>L4-SUM(M2:M3)</f>
+      <c r="L11" s="20">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="N4" s="7">
-        <f>M4-SUM(N2:N3)</f>
+      <c r="M11" s="20">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="O4" s="7">
-        <f>N4-SUM(O2:O3)</f>
+      <c r="N11" s="20">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="P4" s="7">
-        <f>O4-SUM(P2:P3)</f>
+      <c r="O11" s="20">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="Q4" s="7">
-        <f>P4-SUM(Q2:Q3)</f>
+      <c r="P11" s="20">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="R4" s="7">
-        <f>Q4-SUM(R2:R3)</f>
+      <c r="Q11" s="20">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="S4" s="7">
-        <f>R4-SUM(S2:S3)</f>
+      <c r="R11" s="20">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="T4" s="7">
-        <f>S4-SUM(T2:T3)</f>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="9">
+        <f>SUM(C9:C9)</f>
         <v>10</v>
       </c>
-      <c r="U4" s="7">
-        <f>T4-SUM(U2:U3)</f>
-        <v>10</v>
-      </c>
-      <c r="V4" s="7">
-        <f>U4-SUM(V2:V3)</f>
-        <v>10</v>
-      </c>
-      <c r="W4" s="7">
-        <f>V4-SUM(W2:W3)</f>
-        <v>10</v>
-      </c>
-      <c r="X4" s="7">
-        <f>W4-SUM(X2:X3)</f>
-        <v>10</v>
-      </c>
-      <c r="Y4" s="7">
-        <f>X4-SUM(Y2:Y3)</f>
-        <v>10</v>
-      </c>
-      <c r="Z4" s="7">
-        <f>Y4-SUM(Z2:Z3)</f>
-        <v>10</v>
-      </c>
-      <c r="AA4" s="7">
-        <f>Z4-SUM(AA2:AA3)</f>
-        <v>10</v>
-      </c>
-      <c r="AB4" s="7">
-        <f>AA4-SUM(AB2:AB3)</f>
-        <v>10</v>
-      </c>
-      <c r="AC4" s="7">
-        <f>AB4-SUM(AC2:AC3)</f>
-        <v>10</v>
-      </c>
-      <c r="AD4" s="7">
-        <f>AC4-SUM(AD2:AD3)</f>
-        <v>10</v>
-      </c>
-      <c r="AE4" s="7">
-        <f>AD4-SUM(AE2:AE3)</f>
-        <v>10</v>
-      </c>
-      <c r="AF4" s="7">
-        <f>AE4-SUM(AF2:AF3)</f>
-        <v>10</v>
-      </c>
-      <c r="AG4" s="7">
-        <f>AF4-SUM(AG2:AG3)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="11">
-        <f>SUM(C2:C2)</f>
-        <v>10</v>
-      </c>
-      <c r="D5" s="9">
-        <f>C5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>9.6666666666666661</v>
-      </c>
-      <c r="E5" s="9">
-        <f>D5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>9.3333333333333321</v>
-      </c>
-      <c r="F5" s="9">
-        <f>E5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>8.9999999999999982</v>
-      </c>
-      <c r="G5" s="9">
-        <f>F5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>8.6666666666666643</v>
-      </c>
-      <c r="H5" s="9">
-        <f>G5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>8.3333333333333304</v>
-      </c>
-      <c r="I5" s="9">
-        <f>H5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>7.9999999999999973</v>
-      </c>
-      <c r="J5" s="9">
-        <f>I5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>7.6666666666666643</v>
-      </c>
-      <c r="K5" s="9">
-        <f>J5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>7.3333333333333313</v>
-      </c>
-      <c r="L5" s="9">
-        <f>K5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>6.9999999999999982</v>
-      </c>
-      <c r="M5" s="9">
-        <f>L5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>6.6666666666666652</v>
-      </c>
-      <c r="N5" s="9">
-        <f>M5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>6.3333333333333321</v>
-      </c>
-      <c r="O5" s="9">
-        <f>N5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>5.9999999999999991</v>
-      </c>
-      <c r="P5" s="9">
-        <f>O5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>5.6666666666666661</v>
-      </c>
-      <c r="Q5" s="9">
-        <f>P5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>5.333333333333333</v>
-      </c>
-      <c r="R5" s="9">
-        <f>Q5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>5</v>
-      </c>
-      <c r="S5" s="9">
-        <f>R5-($C$5/COUNTA($D$1:$AG$1))</f>
+      <c r="D12" s="17">
+        <f>C12-($C$12/COUNTA($D$1:$R$1))</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="E12" s="17">
+        <f t="shared" ref="E12:R12" si="4">D12-($C$12/COUNTA($D$1:$R$1))</f>
+        <v>8.6666666666666679</v>
+      </c>
+      <c r="F12" s="17">
+        <f t="shared" si="4"/>
+        <v>8.0000000000000018</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" si="4"/>
+        <v>7.3333333333333348</v>
+      </c>
+      <c r="H12" s="17">
+        <f t="shared" si="4"/>
+        <v>6.6666666666666679</v>
+      </c>
+      <c r="I12" s="17">
+        <f t="shared" si="4"/>
+        <v>6.0000000000000009</v>
+      </c>
+      <c r="J12" s="17">
+        <f t="shared" si="4"/>
+        <v>5.3333333333333339</v>
+      </c>
+      <c r="K12" s="17">
+        <f t="shared" si="4"/>
         <v>4.666666666666667</v>
       </c>
-      <c r="T5" s="9">
-        <f>S5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>4.3333333333333339</v>
-      </c>
-      <c r="U5" s="9">
-        <f>T5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>4.0000000000000009</v>
-      </c>
-      <c r="V5" s="9">
-        <f>U5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>3.6666666666666674</v>
-      </c>
-      <c r="W5" s="9">
-        <f>V5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>3.3333333333333339</v>
-      </c>
-      <c r="X5" s="9">
-        <f>W5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>3.0000000000000004</v>
-      </c>
-      <c r="Y5" s="9">
-        <f>X5-($C$5/COUNTA($D$1:$AG$1))</f>
+      <c r="L12" s="17">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="M12" s="17">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="N12" s="17">
+        <f t="shared" si="4"/>
         <v>2.666666666666667</v>
       </c>
-      <c r="Z5" s="9">
-        <f>Y5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>2.3333333333333335</v>
-      </c>
-      <c r="AA5" s="9">
-        <f>Z5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>2</v>
-      </c>
-      <c r="AB5" s="9">
-        <f>AA5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="AC5" s="9">
-        <f>AB5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>1.3333333333333335</v>
-      </c>
-      <c r="AD5" s="9">
-        <f>AC5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>1.0000000000000002</v>
-      </c>
-      <c r="AE5" s="9">
-        <f>AD5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="AF5" s="9">
-        <f>AE5-($C$5/COUNTA($D$1:$AG$1))</f>
-        <v>0.33333333333333365</v>
-      </c>
-      <c r="AG5" s="9">
-        <f>AF5-($C$5/COUNTA($D$1:$AG$1))</f>
+      <c r="O12" s="17">
+        <f t="shared" si="4"/>
+        <v>2.0000000000000004</v>
+      </c>
+      <c r="P12" s="17">
+        <f t="shared" si="4"/>
+        <v>1.3333333333333339</v>
+      </c>
+      <c r="Q12" s="17">
+        <f t="shared" si="4"/>
+        <v>0.6666666666666673</v>
+      </c>
+      <c r="R12" s="17">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A7"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizacao Burndown do Sprint
</commit_message>
<xml_diff>
--- a/academicci_documentacao/gerencia_projeto/Academicci_GBS_BurndownSprint.xlsx
+++ b/academicci_documentacao/gerencia_projeto/Academicci_GBS_BurndownSprint.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>Dia 01</t>
   </si>
@@ -173,6 +173,27 @@
   </si>
   <si>
     <t>Dia 40</t>
+  </si>
+  <si>
+    <t>Definir Framework Back-End</t>
+  </si>
+  <si>
+    <t>Definir Framework Front-End</t>
+  </si>
+  <si>
+    <t>Organizar Gestão de Projeto</t>
+  </si>
+  <si>
+    <t>Documento de Arquitetura</t>
+  </si>
+  <si>
+    <t>Reestruturação do RepositórioAcademicci</t>
+  </si>
+  <si>
+    <t>Treinar Equipe</t>
+  </si>
+  <si>
+    <t>Refinar Documentação do Projeto</t>
   </si>
 </sst>
 </file>
@@ -180,7 +201,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -197,12 +218,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -235,6 +250,12 @@
     </font>
     <font>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="26"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -272,7 +293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -356,65 +377,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +558,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -922,7 +979,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -960,7 +1017,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="778635856"/>
@@ -1043,7 +1100,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1075,7 +1132,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="778639600"/>
@@ -1118,7 +1175,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1148,7 +1205,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1223,7 +1280,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1238,7 +1295,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dados!$B$11</c:f>
+              <c:f>Dados!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1263,54 +1320,54 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Dados!$D$11:$R$11</c:f>
+              <c:f>Dados!$D$17:$R$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>78.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>76.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>72.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1327,7 +1384,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dados!$B$12</c:f>
+              <c:f>Dados!$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1351,51 +1408,51 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Dados!$D$12:$R$12</c:f>
+              <c:f>Dados!$D$18:$R$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>9.3333333333333339</c:v>
+                  <c:v>75.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6666666666666679</c:v>
+                  <c:v>70.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0000000000000018</c:v>
+                  <c:v>64.799999999999983</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.3333333333333348</c:v>
+                  <c:v>59.399999999999984</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.6666666666666679</c:v>
+                  <c:v>53.999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0000000000000009</c:v>
+                  <c:v>48.599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.3333333333333339</c:v>
+                  <c:v>43.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.666666666666667</c:v>
+                  <c:v>37.79999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>32.399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>26.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.666666666666667</c:v>
+                  <c:v>21.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.0000000000000004</c:v>
+                  <c:v>16.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.3333333333333339</c:v>
+                  <c:v>10.799999999999995</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.6666666666666673</c:v>
+                  <c:v>5.399999999999995</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -1494,7 +1551,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1532,7 +1589,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="778635856"/>
@@ -1546,7 +1603,7 @@
         <c:axId val="778635856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="12"/>
+          <c:max val="82"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1615,7 +1672,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1647,13 +1704,13 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="778639600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
+        <c:majorUnit val="4"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1690,7 +1747,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1720,7 +1777,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3176,7 +3233,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
+      <c r="A1" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3189,7 +3246,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3198,7 +3255,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
+      <c r="A1" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3208,16 +3265,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ12"/>
+  <dimension ref="A1:AQ18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="43" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="44" max="63" width="6.28515625" bestFit="1" customWidth="1"/>
@@ -3354,8 +3411,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:43" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:43" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -3409,8 +3466,8 @@
       <c r="AP2" s="4"/>
       <c r="AQ2" s="4"/>
     </row>
-    <row r="3" spans="1:43" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="22"/>
+    <row r="3" spans="1:43" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="20"/>
       <c r="B3" s="3" t="s">
         <v>37</v>
       </c>
@@ -3463,7 +3520,7 @@
       <c r="AQ3" s="4"/>
     </row>
     <row r="4" spans="1:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="3" t="s">
         <v>38</v>
       </c>
@@ -3516,52 +3573,52 @@
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="14"/>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="14"/>
-      <c r="AF5" s="14"/>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="14"/>
-      <c r="AJ5" s="14"/>
-      <c r="AK5" s="14"/>
-      <c r="AL5" s="14"/>
-      <c r="AM5" s="14"/>
-      <c r="AN5" s="14"/>
-      <c r="AO5" s="14"/>
-      <c r="AP5" s="14"/>
-      <c r="AQ5" s="14"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="12"/>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="12"/>
+      <c r="AH5" s="12"/>
+      <c r="AI5" s="12"/>
+      <c r="AJ5" s="12"/>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="12"/>
+      <c r="AM5" s="12"/>
+      <c r="AN5" s="12"/>
+      <c r="AO5" s="12"/>
+      <c r="AP5" s="12"/>
+      <c r="AQ5" s="12"/>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="6" t="s">
         <v>32</v>
       </c>
@@ -3569,525 +3626,724 @@
         <f>SUM(C2:C4)</f>
         <v>23</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="18">
         <f>C6-SUM(D2:D4)</f>
         <v>23</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="18">
         <f t="shared" ref="E6:AG6" si="0">D6-SUM(E2:E4)</f>
         <v>23</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="L6" s="20">
+      <c r="L6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="M6" s="20">
+      <c r="M6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="N6" s="20">
+      <c r="N6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="O6" s="20">
+      <c r="O6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="P6" s="20">
+      <c r="P6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="Q6" s="20">
+      <c r="Q6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="R6" s="20">
+      <c r="R6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="S6" s="20">
+      <c r="S6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="T6" s="20">
+      <c r="T6" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="U6" s="20">
+      <c r="U6" s="18">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="V6" s="20">
+      <c r="V6" s="18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="W6" s="20">
+      <c r="W6" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="X6" s="20">
+      <c r="X6" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="Y6" s="20">
+      <c r="Y6" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="Z6" s="20">
+      <c r="Z6" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="AA6" s="20">
+      <c r="AA6" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="AB6" s="20">
+      <c r="AB6" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="AC6" s="20">
+      <c r="AC6" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="AD6" s="20">
+      <c r="AD6" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="AE6" s="20">
+      <c r="AE6" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="AF6" s="20">
+      <c r="AF6" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="AG6" s="20">
+      <c r="AG6" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="AH6" s="20">
+      <c r="AH6" s="18">
         <f t="shared" ref="AH6:AQ6" si="1">AG6-SUM(AH2:AH4)</f>
         <v>12</v>
       </c>
-      <c r="AI6" s="20">
+      <c r="AI6" s="18">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="AJ6" s="20">
+      <c r="AJ6" s="18">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="AK6" s="20">
+      <c r="AK6" s="18">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="AL6" s="20">
+      <c r="AL6" s="18">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="AM6" s="20">
+      <c r="AM6" s="18">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="AN6" s="20">
+      <c r="AN6" s="18">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="AO6" s="20">
+      <c r="AO6" s="18">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="AP6" s="20">
+      <c r="AP6" s="18">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="AQ6" s="20">
+      <c r="AQ6" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="17">
         <v>23</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <f>C7-($C$7/COUNTA($D$1:$AQ$1))</f>
         <v>22.425000000000001</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <f t="shared" ref="E7:AQ7" si="2">D7-($C$7/COUNTA($D$1:$AQ$1))</f>
         <v>21.85</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="16">
         <f t="shared" si="2"/>
         <v>21.275000000000002</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="16">
         <f t="shared" si="2"/>
         <v>20.700000000000003</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="16">
         <f t="shared" si="2"/>
         <v>20.125000000000004</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="16">
         <f t="shared" si="2"/>
         <v>19.550000000000004</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="16">
         <f t="shared" si="2"/>
         <v>18.975000000000005</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="16">
         <f t="shared" si="2"/>
         <v>18.400000000000006</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="16">
         <f t="shared" si="2"/>
         <v>17.825000000000006</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="16">
         <f t="shared" si="2"/>
         <v>17.250000000000007</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="16">
         <f t="shared" si="2"/>
         <v>16.675000000000008</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="16">
         <f t="shared" si="2"/>
         <v>16.100000000000009</v>
       </c>
-      <c r="P7" s="18">
+      <c r="P7" s="16">
         <f t="shared" si="2"/>
         <v>15.525000000000009</v>
       </c>
-      <c r="Q7" s="18">
+      <c r="Q7" s="16">
         <f t="shared" si="2"/>
         <v>14.95000000000001</v>
       </c>
-      <c r="R7" s="18">
+      <c r="R7" s="16">
         <f t="shared" si="2"/>
         <v>14.375000000000011</v>
       </c>
-      <c r="S7" s="18">
+      <c r="S7" s="16">
         <f t="shared" si="2"/>
         <v>13.800000000000011</v>
       </c>
-      <c r="T7" s="18">
+      <c r="T7" s="16">
         <f t="shared" si="2"/>
         <v>13.225000000000012</v>
       </c>
-      <c r="U7" s="18">
+      <c r="U7" s="16">
         <f t="shared" si="2"/>
         <v>12.650000000000013</v>
       </c>
-      <c r="V7" s="18">
+      <c r="V7" s="16">
         <f t="shared" si="2"/>
         <v>12.075000000000014</v>
       </c>
-      <c r="W7" s="18">
+      <c r="W7" s="16">
         <f t="shared" si="2"/>
         <v>11.500000000000014</v>
       </c>
-      <c r="X7" s="18">
+      <c r="X7" s="16">
         <f t="shared" si="2"/>
         <v>10.925000000000015</v>
       </c>
-      <c r="Y7" s="18">
+      <c r="Y7" s="16">
         <f t="shared" si="2"/>
         <v>10.350000000000016</v>
       </c>
-      <c r="Z7" s="18">
+      <c r="Z7" s="16">
         <f t="shared" si="2"/>
         <v>9.7750000000000163</v>
       </c>
-      <c r="AA7" s="18">
+      <c r="AA7" s="16">
         <f t="shared" si="2"/>
         <v>9.2000000000000171</v>
       </c>
-      <c r="AB7" s="18">
+      <c r="AB7" s="16">
         <f t="shared" si="2"/>
         <v>8.6250000000000178</v>
       </c>
-      <c r="AC7" s="18">
+      <c r="AC7" s="16">
         <f t="shared" si="2"/>
         <v>8.0500000000000185</v>
       </c>
-      <c r="AD7" s="18">
+      <c r="AD7" s="16">
         <f t="shared" si="2"/>
         <v>7.4750000000000183</v>
       </c>
-      <c r="AE7" s="18">
+      <c r="AE7" s="16">
         <f t="shared" si="2"/>
         <v>6.9000000000000181</v>
       </c>
-      <c r="AF7" s="18">
+      <c r="AF7" s="16">
         <f t="shared" si="2"/>
         <v>6.3250000000000179</v>
       </c>
-      <c r="AG7" s="18">
+      <c r="AG7" s="16">
         <f t="shared" si="2"/>
         <v>5.7500000000000178</v>
       </c>
-      <c r="AH7" s="18">
+      <c r="AH7" s="16">
         <f t="shared" si="2"/>
         <v>5.1750000000000176</v>
       </c>
-      <c r="AI7" s="18">
+      <c r="AI7" s="16">
         <f t="shared" si="2"/>
         <v>4.6000000000000174</v>
       </c>
-      <c r="AJ7" s="18">
+      <c r="AJ7" s="16">
         <f t="shared" si="2"/>
         <v>4.0250000000000172</v>
       </c>
-      <c r="AK7" s="18">
+      <c r="AK7" s="16">
         <f t="shared" si="2"/>
         <v>3.4500000000000171</v>
       </c>
-      <c r="AL7" s="18">
+      <c r="AL7" s="16">
         <f t="shared" si="2"/>
         <v>2.8750000000000169</v>
       </c>
-      <c r="AM7" s="18">
+      <c r="AM7" s="16">
         <f t="shared" si="2"/>
         <v>2.3000000000000167</v>
       </c>
-      <c r="AN7" s="18">
+      <c r="AN7" s="16">
         <f t="shared" si="2"/>
         <v>1.7250000000000167</v>
       </c>
-      <c r="AO7" s="18">
+      <c r="AO7" s="16">
         <f t="shared" si="2"/>
         <v>1.1500000000000168</v>
       </c>
-      <c r="AP7" s="18">
+      <c r="AP7" s="16">
         <f t="shared" si="2"/>
         <v>0.57500000000001683</v>
       </c>
-      <c r="AQ7" s="18">
+      <c r="AQ7" s="16">
         <f t="shared" si="2"/>
         <v>1.6875389974302379E-14</v>
       </c>
     </row>
-    <row r="9" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C9" s="10">
-        <v>10</v>
+        <v>6.5</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4">
+        <v>0.5</v>
+      </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="O9" s="4">
+        <v>8</v>
+      </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4">
+        <v>2</v>
+      </c>
+      <c r="N10" s="4">
+        <v>2</v>
+      </c>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="8">
-        <f>SUM(C9:C9)</f>
-        <v>10</v>
-      </c>
-      <c r="D11" s="20">
-        <f>C11-SUM(D9)</f>
-        <v>10</v>
-      </c>
-      <c r="E11" s="20">
-        <f t="shared" ref="E11:R11" si="3">D11-SUM(E9)</f>
-        <v>10</v>
-      </c>
-      <c r="F11" s="20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="G11" s="20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H11" s="20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="I11" s="20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="J11" s="20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="K11" s="20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="L11" s="20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="M11" s="20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="N11" s="20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="O11" s="20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="P11" s="20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="Q11" s="20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="R11" s="20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
+      <c r="A11" s="24"/>
+      <c r="B11" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="10">
+        <v>13</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4">
+        <v>2</v>
+      </c>
+      <c r="M11" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="N11" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="O11" s="4">
+        <v>1</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="24"/>
+      <c r="B12" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="10">
+        <v>12</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="10">
+        <v>12.5</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4">
+        <v>4</v>
+      </c>
+      <c r="J13" s="4">
+        <v>3</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2</v>
+      </c>
+      <c r="L13" s="4">
+        <v>3</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="10">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4">
+        <v>3</v>
+      </c>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="10">
+        <v>30</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4">
+        <v>2</v>
+      </c>
+      <c r="F15" s="4">
+        <v>2</v>
+      </c>
+      <c r="G15" s="4">
+        <v>2</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2</v>
+      </c>
+      <c r="J15" s="4">
+        <v>4</v>
+      </c>
+      <c r="K15" s="4">
+        <v>3</v>
+      </c>
+      <c r="L15" s="4">
+        <v>3</v>
+      </c>
+      <c r="M15" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="N15" s="4">
+        <v>2</v>
+      </c>
+      <c r="O15" s="4">
+        <v>1</v>
+      </c>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="8">
+        <f>SUM(C9:C15)</f>
+        <v>81</v>
+      </c>
+      <c r="D17" s="18">
+        <f>C17-SUM(D9:D15)</f>
+        <v>81</v>
+      </c>
+      <c r="E17" s="18">
+        <f t="shared" ref="E17:R17" si="3">D17-SUM(E9:E15)</f>
+        <v>78.5</v>
+      </c>
+      <c r="F17" s="18">
+        <f t="shared" si="3"/>
+        <v>76.5</v>
+      </c>
+      <c r="G17" s="18">
+        <f t="shared" si="3"/>
+        <v>74.5</v>
+      </c>
+      <c r="H17" s="18">
+        <f t="shared" si="3"/>
+        <v>72.5</v>
+      </c>
+      <c r="I17" s="18">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="J17" s="18">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="K17" s="18">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="L17" s="18">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="M17" s="18">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="N17" s="18">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="O17" s="18">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="P17" s="18">
+        <f t="shared" si="3"/>
+        <v>14.5</v>
+      </c>
+      <c r="Q17" s="18">
+        <f t="shared" si="3"/>
+        <v>14.5</v>
+      </c>
+      <c r="R17" s="18">
+        <f t="shared" si="3"/>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="9">
-        <f>SUM(C9:C9)</f>
-        <v>10</v>
-      </c>
-      <c r="D12" s="17">
-        <f>C12-($C$12/COUNTA($D$1:$R$1))</f>
-        <v>9.3333333333333339</v>
-      </c>
-      <c r="E12" s="17">
-        <f t="shared" ref="E12:R12" si="4">D12-($C$12/COUNTA($D$1:$R$1))</f>
-        <v>8.6666666666666679</v>
-      </c>
-      <c r="F12" s="17">
-        <f t="shared" si="4"/>
-        <v>8.0000000000000018</v>
-      </c>
-      <c r="G12" s="17">
-        <f t="shared" si="4"/>
-        <v>7.3333333333333348</v>
-      </c>
-      <c r="H12" s="17">
-        <f t="shared" si="4"/>
-        <v>6.6666666666666679</v>
-      </c>
-      <c r="I12" s="17">
-        <f t="shared" si="4"/>
-        <v>6.0000000000000009</v>
-      </c>
-      <c r="J12" s="17">
-        <f t="shared" si="4"/>
-        <v>5.3333333333333339</v>
-      </c>
-      <c r="K12" s="17">
-        <f t="shared" si="4"/>
-        <v>4.666666666666667</v>
-      </c>
-      <c r="L12" s="17">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="M12" s="17">
-        <f t="shared" si="4"/>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="N12" s="17">
-        <f t="shared" si="4"/>
-        <v>2.666666666666667</v>
-      </c>
-      <c r="O12" s="17">
-        <f t="shared" si="4"/>
-        <v>2.0000000000000004</v>
-      </c>
-      <c r="P12" s="17">
-        <f t="shared" si="4"/>
-        <v>1.3333333333333339</v>
-      </c>
-      <c r="Q12" s="17">
-        <f t="shared" si="4"/>
-        <v>0.6666666666666673</v>
-      </c>
-      <c r="R12" s="17">
-        <f t="shared" si="4"/>
+      <c r="C18" s="9">
+        <f>SUM(C9:C15)</f>
+        <v>81</v>
+      </c>
+      <c r="D18" s="15">
+        <f>C18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>75.599999999999994</v>
+      </c>
+      <c r="E18" s="15">
+        <f>D18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>70.199999999999989</v>
+      </c>
+      <c r="F18" s="15">
+        <f>E18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>64.799999999999983</v>
+      </c>
+      <c r="G18" s="15">
+        <f>F18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>59.399999999999984</v>
+      </c>
+      <c r="H18" s="15">
+        <f>G18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>53.999999999999986</v>
+      </c>
+      <c r="I18" s="15">
+        <f>H18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>48.599999999999987</v>
+      </c>
+      <c r="J18" s="15">
+        <f>I18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>43.199999999999989</v>
+      </c>
+      <c r="K18" s="15">
+        <f>J18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>37.79999999999999</v>
+      </c>
+      <c r="L18" s="15">
+        <f>K18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>32.399999999999991</v>
+      </c>
+      <c r="M18" s="15">
+        <f>L18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>26.999999999999993</v>
+      </c>
+      <c r="N18" s="15">
+        <f>M18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>21.599999999999994</v>
+      </c>
+      <c r="O18" s="15">
+        <f>N18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>16.199999999999996</v>
+      </c>
+      <c r="P18" s="15">
+        <f>O18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>10.799999999999995</v>
+      </c>
+      <c r="Q18" s="15">
+        <f>P18-($C$18/COUNTA($D$1:$R$1))</f>
+        <v>5.399999999999995</v>
+      </c>
+      <c r="R18" s="15">
+        <f>Q18-($C$18/COUNTA($D$1:$R$1))</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A9:A18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizacao de arquivos e planejamento de sprint 003
</commit_message>
<xml_diff>
--- a/academicci_documentacao/gerencia_projeto/Academicci_GBS_BurndownSprint.xlsx
+++ b/academicci_documentacao/gerencia_projeto/Academicci_GBS_BurndownSprint.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\Google Drive\University - Atividades e Trabalhos\PFS_II\Academicci_II\academicci_documentacao\gerencia_projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttava\OneDrive\Documents\Engenharia de Computação\9ºPERIODO\PRATICA EM FABRICA DE SOFTWARE II\Academicci_II\academicci_documentacao\gerencia_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_9277B3099DB60CEC1FB7B39C605C683879EDAEF5" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7770" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint01" sheetId="2" r:id="rId1"/>
     <sheet name="Sprint02" sheetId="3" r:id="rId2"/>
     <sheet name="Dados" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -199,7 +200,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -452,6 +453,8 @@
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -461,7 +464,6 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -471,7 +473,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,7 +559,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -979,7 +980,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1017,7 +1018,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="778635856"/>
@@ -1100,7 +1101,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1132,7 +1133,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="778639600"/>
@@ -1175,7 +1176,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1205,7 +1206,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1280,7 +1281,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1551,7 +1552,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1589,7 +1590,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="778635856"/>
@@ -1672,7 +1673,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1704,7 +1705,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="778639600"/>
@@ -1747,7 +1748,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1777,7 +1778,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3220,7 +3221,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3242,7 +3243,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -3264,7 +3265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AQ18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -3412,7 +3413,7 @@
       </c>
     </row>
     <row r="2" spans="1:43" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -3467,7 +3468,7 @@
       <c r="AQ2" s="4"/>
     </row>
     <row r="3" spans="1:43" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="3" t="s">
         <v>37</v>
       </c>
@@ -3520,7 +3521,7 @@
       <c r="AQ3" s="4"/>
     </row>
     <row r="4" spans="1:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="3" t="s">
         <v>38</v>
       </c>
@@ -3573,7 +3574,7 @@
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -3618,7 +3619,7 @@
       <c r="AQ5" s="12"/>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="6" t="s">
         <v>32</v>
       </c>
@@ -3788,7 +3789,7 @@
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="7" t="s">
         <v>33</v>
       </c>
@@ -3957,7 +3958,7 @@
       </c>
     </row>
     <row r="9" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="24" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -3987,8 +3988,8 @@
       <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="22" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="19" t="s">
         <v>50</v>
       </c>
       <c r="C10" s="10">
@@ -4015,8 +4016,8 @@
       <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="22" t="s">
+      <c r="A11" s="25"/>
+      <c r="B11" s="19" t="s">
         <v>51</v>
       </c>
       <c r="C11" s="10">
@@ -4051,8 +4052,8 @@
       <c r="R11" s="4"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="19" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="10">
@@ -4075,8 +4076,8 @@
       <c r="R12" s="4"/>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="22" t="s">
+      <c r="A13" s="25"/>
+      <c r="B13" s="19" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="10">
@@ -4109,8 +4110,8 @@
       <c r="R13" s="4"/>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="26" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="20" t="s">
         <v>55</v>
       </c>
       <c r="C14" s="10">
@@ -4135,8 +4136,8 @@
       <c r="R14" s="4"/>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="26" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="20" t="s">
         <v>54</v>
       </c>
       <c r="C15" s="10">
@@ -4181,7 +4182,7 @@
       <c r="R15" s="4"/>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -4201,7 +4202,7 @@
       <c r="R16" s="12"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="6" t="s">
         <v>32</v>
       </c>
@@ -4271,7 +4272,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="7" t="s">
         <v>33</v>
       </c>
@@ -4280,63 +4281,63 @@
         <v>81</v>
       </c>
       <c r="D18" s="15">
-        <f>C18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" ref="D18:R18" si="4">C18-($C$18/COUNTA($D$1:$R$1))</f>
         <v>75.599999999999994</v>
       </c>
       <c r="E18" s="15">
-        <f>D18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>70.199999999999989</v>
       </c>
       <c r="F18" s="15">
-        <f>E18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>64.799999999999983</v>
       </c>
       <c r="G18" s="15">
-        <f>F18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>59.399999999999984</v>
       </c>
       <c r="H18" s="15">
-        <f>G18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>53.999999999999986</v>
       </c>
       <c r="I18" s="15">
-        <f>H18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>48.599999999999987</v>
       </c>
       <c r="J18" s="15">
-        <f>I18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>43.199999999999989</v>
       </c>
       <c r="K18" s="15">
-        <f>J18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>37.79999999999999</v>
       </c>
       <c r="L18" s="15">
-        <f>K18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>32.399999999999991</v>
       </c>
       <c r="M18" s="15">
-        <f>L18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>26.999999999999993</v>
       </c>
       <c r="N18" s="15">
-        <f>M18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>21.599999999999994</v>
       </c>
       <c r="O18" s="15">
-        <f>N18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>16.199999999999996</v>
       </c>
       <c r="P18" s="15">
-        <f>O18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>10.799999999999995</v>
       </c>
       <c r="Q18" s="15">
-        <f>P18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>5.399999999999995</v>
       </c>
       <c r="R18" s="15">
-        <f>Q18-($C$18/COUNTA($D$1:$R$1))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizacao Burndown do Sprint 03
</commit_message>
<xml_diff>
--- a/academicci_documentacao/gerencia_projeto/Academicci_GBS_BurndownSprint.xlsx
+++ b/academicci_documentacao/gerencia_projeto/Academicci_GBS_BurndownSprint.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttava\OneDrive\Documents\Engenharia de Computação\9ºPERIODO\PRATICA EM FABRICA DE SOFTWARE II\Academicci_II\academicci_documentacao\gerencia_projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\Google Drive\University - 002 Atividades e Trabalhos\PFS_II\Academicci_II\academicci_documentacao\gerencia_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_9277B3099DB60CEC1FB7B39C605C683879EDAEF5" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7770" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7770" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint01" sheetId="2" r:id="rId1"/>
     <sheet name="Sprint02" sheetId="3" r:id="rId2"/>
-    <sheet name="Dados" sheetId="1" r:id="rId3"/>
+    <sheet name="Sprint03" sheetId="4" r:id="rId3"/>
+    <sheet name="Dados" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
   <si>
     <t>Dia 01</t>
   </si>
@@ -195,12 +195,42 @@
   </si>
   <si>
     <t>Refinar Documentação do Projeto</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Refinar Documento de Arquitetura</t>
+  </si>
+  <si>
+    <t>Criar Disciplina</t>
+  </si>
+  <si>
+    <t>Editar Disciplina</t>
+  </si>
+  <si>
+    <t>Listar Disciplina</t>
+  </si>
+  <si>
+    <t>Autenticar Usuário</t>
+  </si>
+  <si>
+    <t>Editar Usuário</t>
+  </si>
+  <si>
+    <t>Aitvar Disciplina</t>
+  </si>
+  <si>
+    <t>Destaviar Disciplina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -559,7 +589,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -980,7 +1010,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1018,7 +1048,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="778635856"/>
@@ -1101,7 +1131,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1133,7 +1163,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="778639600"/>
@@ -1176,7 +1206,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1206,7 +1236,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1281,7 +1311,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1552,7 +1582,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1590,7 +1620,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="778635856"/>
@@ -1673,7 +1703,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1705,7 +1735,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="778639600"/>
@@ -1748,7 +1778,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1778,7 +1808,579 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Gráfico BurnDown - Sprint 03</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dados!$B$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Restantes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Dados!$D$30:$R$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FD19-4386-934C-DBF33CA211DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dados!$B$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Estimadas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Dados!$D$31:$R$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>22.866666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.233333333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.966666666666669</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.333333333333336</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.06666666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.433333333333337</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.8000000000000043</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.1666666666666714</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.5333333333333385</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.9000000000000057</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.2666666666666724</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6333333333333391</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.773159728050814E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FD19-4386-934C-DBF33CA211DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="778639600"/>
+        <c:axId val="778635856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="778639600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" b="1">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Dias</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="778635856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="778635856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="82"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" b="1">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Hoaras</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="778639600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1869,6 +2471,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2373,6 +3015,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2937,6 +4082,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACFE61B1-19C7-4FED-A857-23140CA48041}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180973</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{636C56C6-908F-4B79-9850-05F273683FE8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3221,7 +4409,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3243,10 +4431,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
@@ -3265,11 +4453,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AQ18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AQ31"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3959,7 +5169,7 @@
     </row>
     <row r="9" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>49</v>
@@ -4341,10 +5551,389 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="10">
+        <v>12</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+    </row>
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="10">
+        <v>4.75</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+    </row>
+    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+      <c r="B22" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="10">
+        <v>4.75</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+    </row>
+    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
+      <c r="B25" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+      <c r="B26" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="25"/>
+      <c r="B28" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="8">
+        <f>SUM(C20:C28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="D30" s="18">
+        <f>C30-SUM(D20:D28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="E30" s="18">
+        <f>D30-SUM(E20:E28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="F30" s="18">
+        <f>E30-SUM(F20:F28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="G30" s="18">
+        <f>F30-SUM(G20:G28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="H30" s="18">
+        <f>G30-SUM(H20:H28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="I30" s="18">
+        <f>H30-SUM(I20:I28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="J30" s="18">
+        <f>I30-SUM(J20:J28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="K30" s="18">
+        <f>J30-SUM(K20:K28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="L30" s="18">
+        <f>K30-SUM(L20:L28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="M30" s="18">
+        <f>L30-SUM(M20:M28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="N30" s="18">
+        <f>M30-SUM(N20:N28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="O30" s="18">
+        <f>N30-SUM(O20:O28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="P30" s="18">
+        <f>O30-SUM(P20:P28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="Q30" s="18">
+        <f>P30-SUM(Q20:Q28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="R30" s="18">
+        <f>Q30-SUM(R20:R28)</f>
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="9">
+        <f>SUM(C20:C28)</f>
+        <v>24.5</v>
+      </c>
+      <c r="D31" s="15">
+        <f>C31-($C$31/COUNTA($D$1:$R$1))</f>
+        <v>22.866666666666667</v>
+      </c>
+      <c r="E31" s="15">
+        <f t="shared" ref="E31:R31" si="5">D31-($C$31/COUNTA($D$1:$R$1))</f>
+        <v>21.233333333333334</v>
+      </c>
+      <c r="F31" s="15">
+        <f t="shared" si="5"/>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="G31" s="15">
+        <f t="shared" si="5"/>
+        <v>17.966666666666669</v>
+      </c>
+      <c r="H31" s="15">
+        <f t="shared" si="5"/>
+        <v>16.333333333333336</v>
+      </c>
+      <c r="I31" s="15">
+        <f t="shared" si="5"/>
+        <v>14.700000000000003</v>
+      </c>
+      <c r="J31" s="15">
+        <f t="shared" si="5"/>
+        <v>13.06666666666667</v>
+      </c>
+      <c r="K31" s="15">
+        <f t="shared" si="5"/>
+        <v>11.433333333333337</v>
+      </c>
+      <c r="L31" s="15">
+        <f t="shared" si="5"/>
+        <v>9.8000000000000043</v>
+      </c>
+      <c r="M31" s="15">
+        <f t="shared" si="5"/>
+        <v>8.1666666666666714</v>
+      </c>
+      <c r="N31" s="15">
+        <f t="shared" si="5"/>
+        <v>6.5333333333333385</v>
+      </c>
+      <c r="O31" s="15">
+        <f t="shared" si="5"/>
+        <v>4.9000000000000057</v>
+      </c>
+      <c r="P31" s="15">
+        <f t="shared" si="5"/>
+        <v>3.2666666666666724</v>
+      </c>
+      <c r="Q31" s="15">
+        <f t="shared" si="5"/>
+        <v>1.6333333333333391</v>
+      </c>
+      <c r="R31" s="15">
+        <f t="shared" si="5"/>
+        <v>5.773159728050814E-15</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A9:A18"/>
+    <mergeCell ref="A20:A31"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>